<commit_message>
Priya worked on vendor list
</commit_message>
<xml_diff>
--- a/Documents/Test Website/supermarket_Product_List.xlsx
+++ b/Documents/Test Website/supermarket_Product_List.xlsx
@@ -6606,8 +6606,8 @@
   </sheetPr>
   <dimension ref="A1:AB376"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J376" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3:Q376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6770,6 +6770,9 @@
       <c r="P2" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q2" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T2" s="7" t="s">
         <v>37</v>
       </c>
@@ -6823,6 +6826,9 @@
       <c r="P3" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q3" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T3" s="7" t="s">
         <v>41</v>
       </c>
@@ -6878,7 +6884,9 @@
       <c r="P4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" s="7"/>
+      <c r="Q4" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7" t="s">
@@ -6941,7 +6949,9 @@
       <c r="P5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7" t="s">
@@ -7004,7 +7014,9 @@
       <c r="P6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" s="7"/>
+      <c r="Q6" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7" t="s">
@@ -7067,7 +7079,9 @@
       <c r="P7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="7"/>
+      <c r="Q7" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7" t="s">
@@ -7130,7 +7144,9 @@
       <c r="P8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="7"/>
+      <c r="Q8" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7" t="s">
@@ -7193,7 +7209,9 @@
       <c r="P9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="7"/>
+      <c r="Q9" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7" t="s">
@@ -7256,7 +7274,9 @@
       <c r="P10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" s="7"/>
+      <c r="Q10" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7" t="s">
@@ -7317,6 +7337,9 @@
       <c r="P11" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q11" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T11" s="7" t="s">
         <v>50</v>
       </c>
@@ -7370,6 +7393,9 @@
       <c r="P12" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q12" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T12" s="7" t="s">
         <v>89</v>
       </c>
@@ -7423,6 +7449,9 @@
       <c r="P13" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q13" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T13" s="2" t="s">
         <v>94</v>
       </c>
@@ -7476,6 +7505,9 @@
       <c r="P14" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q14" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T14" s="2" t="s">
         <v>94</v>
       </c>
@@ -7529,6 +7561,9 @@
       <c r="P15" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q15" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T15" s="2" t="s">
         <v>103</v>
       </c>
@@ -7582,6 +7617,9 @@
       <c r="P16" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q16" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T16" s="2" t="s">
         <v>103</v>
       </c>
@@ -7635,6 +7673,9 @@
       <c r="P17" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q17" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T17" s="2" t="s">
         <v>103</v>
       </c>
@@ -7688,6 +7729,9 @@
       <c r="P18" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q18" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T18" s="2" t="s">
         <v>113</v>
       </c>
@@ -7741,6 +7785,9 @@
       <c r="P19" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q19" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T19" s="2" t="s">
         <v>120</v>
       </c>
@@ -7794,6 +7841,9 @@
       <c r="P20" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q20" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T20" s="2" t="s">
         <v>113</v>
       </c>
@@ -7847,6 +7897,9 @@
       <c r="P21" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q21" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T21" s="2" t="s">
         <v>127</v>
       </c>
@@ -7900,6 +7953,9 @@
       <c r="P22" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q22" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T22" s="2" t="s">
         <v>133</v>
       </c>
@@ -7953,6 +8009,9 @@
       <c r="P23" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q23" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T23" s="2" t="s">
         <v>138</v>
       </c>
@@ -8006,6 +8065,9 @@
       <c r="P24" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q24" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T24" s="2" t="s">
         <v>145</v>
       </c>
@@ -8059,6 +8121,9 @@
       <c r="P25" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q25" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T25" s="2" t="s">
         <v>153</v>
       </c>
@@ -8112,6 +8177,9 @@
       <c r="P26" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q26" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T26" s="2" t="s">
         <v>156</v>
       </c>
@@ -8165,6 +8233,9 @@
       <c r="P27" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q27" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T27" s="2" t="s">
         <v>158</v>
       </c>
@@ -8215,6 +8286,9 @@
       <c r="P28" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q28" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T28" s="2" t="s">
         <v>162</v>
       </c>
@@ -8267,6 +8341,9 @@
       </c>
       <c r="P29" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="Q29" s="2" t="n">
+        <v>999999</v>
       </c>
       <c r="T29" s="2" t="s">
         <v>167</v>
@@ -8321,6 +8398,9 @@
       <c r="P30" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q30" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T30" s="2" t="s">
         <v>173</v>
       </c>
@@ -8374,6 +8454,9 @@
       <c r="P31" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q31" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T31" s="2" t="s">
         <v>179</v>
       </c>
@@ -8427,6 +8510,9 @@
       <c r="P32" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q32" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T32" s="2" t="s">
         <v>173</v>
       </c>
@@ -8480,6 +8566,9 @@
       <c r="P33" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q33" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T33" s="2" t="s">
         <v>156</v>
       </c>
@@ -8533,6 +8622,9 @@
       <c r="P34" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q34" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T34" s="2" t="s">
         <v>156</v>
       </c>
@@ -8586,6 +8678,9 @@
       <c r="P35" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q35" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T35" s="2" t="s">
         <v>156</v>
       </c>
@@ -8639,6 +8734,9 @@
       <c r="P36" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q36" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T36" s="2" t="s">
         <v>156</v>
       </c>
@@ -8691,6 +8789,9 @@
       </c>
       <c r="P37" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="Q37" s="2" t="n">
+        <v>999999</v>
       </c>
       <c r="T37" s="2" t="s">
         <v>156</v>
@@ -8745,6 +8846,9 @@
       <c r="P38" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q38" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T38" s="2" t="s">
         <v>215</v>
       </c>
@@ -8798,6 +8902,9 @@
       <c r="P39" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q39" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T39" s="2" t="s">
         <v>156</v>
       </c>
@@ -8851,6 +8958,9 @@
       <c r="P40" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q40" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T40" s="2" t="s">
         <v>156</v>
       </c>
@@ -8904,6 +9014,9 @@
       <c r="P41" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q41" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T41" s="2" t="s">
         <v>156</v>
       </c>
@@ -8957,6 +9070,9 @@
       <c r="P42" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q42" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T42" s="2" t="s">
         <v>156</v>
       </c>
@@ -9010,6 +9126,9 @@
       <c r="P43" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q43" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T43" s="2" t="s">
         <v>153</v>
       </c>
@@ -9063,6 +9182,9 @@
       <c r="P44" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q44" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T44" s="2" t="s">
         <v>156</v>
       </c>
@@ -9116,6 +9238,9 @@
       <c r="P45" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q45" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T45" s="2" t="s">
         <v>156</v>
       </c>
@@ -9169,6 +9294,9 @@
       <c r="P46" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q46" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T46" s="2" t="s">
         <v>156</v>
       </c>
@@ -9222,6 +9350,9 @@
       <c r="P47" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q47" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T47" s="2" t="s">
         <v>120</v>
       </c>
@@ -9275,6 +9406,9 @@
       <c r="P48" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q48" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T48" s="2" t="s">
         <v>173</v>
       </c>
@@ -9328,6 +9462,9 @@
       <c r="P49" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q49" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T49" s="2" t="s">
         <v>267</v>
       </c>
@@ -9381,6 +9518,9 @@
       <c r="P50" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q50" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T50" s="2" t="s">
         <v>273</v>
       </c>
@@ -9434,6 +9574,9 @@
       <c r="P51" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q51" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T51" s="2" t="s">
         <v>278</v>
       </c>
@@ -9487,6 +9630,9 @@
       <c r="P52" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q52" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T52" s="2" t="s">
         <v>156</v>
       </c>
@@ -9540,6 +9686,9 @@
       <c r="P53" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q53" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T53" s="2" t="s">
         <v>156</v>
       </c>
@@ -9593,6 +9742,9 @@
       <c r="P54" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q54" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T54" s="2" t="s">
         <v>120</v>
       </c>
@@ -9646,6 +9798,9 @@
       <c r="P55" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q55" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T55" s="2" t="s">
         <v>120</v>
       </c>
@@ -9699,6 +9854,9 @@
       <c r="P56" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q56" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T56" s="2" t="s">
         <v>301</v>
       </c>
@@ -9752,6 +9910,9 @@
       <c r="P57" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q57" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T57" s="2" t="s">
         <v>267</v>
       </c>
@@ -9805,6 +9966,9 @@
       <c r="P58" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q58" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T58" s="2" t="s">
         <v>267</v>
       </c>
@@ -9858,6 +10022,9 @@
       <c r="P59" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q59" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T59" s="2" t="s">
         <v>267</v>
       </c>
@@ -9911,6 +10078,9 @@
       <c r="P60" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q60" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T60" s="2" t="s">
         <v>173</v>
       </c>
@@ -9964,6 +10134,9 @@
       <c r="P61" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q61" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T61" s="2" t="s">
         <v>156</v>
       </c>
@@ -10017,6 +10190,9 @@
       <c r="P62" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q62" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T62" s="2" t="s">
         <v>173</v>
       </c>
@@ -10070,6 +10246,9 @@
       <c r="P63" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q63" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T63" s="2" t="s">
         <v>173</v>
       </c>
@@ -10123,6 +10302,9 @@
       <c r="P64" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q64" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T64" s="2" t="s">
         <v>173</v>
       </c>
@@ -10176,6 +10358,9 @@
       <c r="P65" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q65" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T65" s="2" t="s">
         <v>156</v>
       </c>
@@ -10229,6 +10414,9 @@
       <c r="P66" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q66" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T66" s="2" t="s">
         <v>348</v>
       </c>
@@ -10282,6 +10470,9 @@
       <c r="P67" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q67" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T67" s="2" t="s">
         <v>113</v>
       </c>
@@ -10332,6 +10523,9 @@
       <c r="P68" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q68" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T68" s="2" t="s">
         <v>138</v>
       </c>
@@ -10382,6 +10576,9 @@
       <c r="P69" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q69" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T69" s="2" t="s">
         <v>358</v>
       </c>
@@ -10432,6 +10629,9 @@
       <c r="P70" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q70" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T70" s="2" t="s">
         <v>363</v>
       </c>
@@ -10485,6 +10685,9 @@
       <c r="P71" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q71" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T71" s="2" t="s">
         <v>370</v>
       </c>
@@ -10538,6 +10741,9 @@
       <c r="P72" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q72" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T72" s="2" t="s">
         <v>373</v>
       </c>
@@ -10591,6 +10797,9 @@
       <c r="P73" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q73" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T73" s="2" t="s">
         <v>138</v>
       </c>
@@ -10644,6 +10853,9 @@
       <c r="P74" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q74" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T74" s="2" t="s">
         <v>113</v>
       </c>
@@ -10697,6 +10909,9 @@
       <c r="P75" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q75" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T75" s="2" t="s">
         <v>133</v>
       </c>
@@ -10750,6 +10965,9 @@
       <c r="P76" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q76" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T76" s="2" t="s">
         <v>138</v>
       </c>
@@ -10803,6 +11021,9 @@
       <c r="P77" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q77" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T77" s="2" t="s">
         <v>398</v>
       </c>
@@ -10856,6 +11077,9 @@
       <c r="P78" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q78" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T78" s="2" t="s">
         <v>133</v>
       </c>
@@ -10909,6 +11133,9 @@
       <c r="P79" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q79" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T79" s="2" t="s">
         <v>133</v>
       </c>
@@ -10962,6 +11189,9 @@
       <c r="P80" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q80" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T80" s="2" t="s">
         <v>133</v>
       </c>
@@ -11015,6 +11245,9 @@
       <c r="P81" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q81" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T81" s="2" t="s">
         <v>158</v>
       </c>
@@ -11068,6 +11301,9 @@
       <c r="P82" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q82" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T82" s="2" t="s">
         <v>120</v>
       </c>
@@ -11121,6 +11357,9 @@
       <c r="P83" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q83" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T83" s="2" t="s">
         <v>428</v>
       </c>
@@ -11174,6 +11413,9 @@
       <c r="P84" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q84" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T84" s="2" t="s">
         <v>434</v>
       </c>
@@ -11227,6 +11469,9 @@
       <c r="P85" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q85" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T85" s="2" t="s">
         <v>440</v>
       </c>
@@ -11280,6 +11525,9 @@
       <c r="P86" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q86" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T86" s="2" t="s">
         <v>448</v>
       </c>
@@ -11333,6 +11581,9 @@
       <c r="P87" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q87" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T87" s="2" t="s">
         <v>138</v>
       </c>
@@ -11386,6 +11637,9 @@
       <c r="P88" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q88" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T88" s="2" t="s">
         <v>448</v>
       </c>
@@ -11439,6 +11693,9 @@
       <c r="P89" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q89" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T89" s="2" t="s">
         <v>138</v>
       </c>
@@ -11492,6 +11749,9 @@
       <c r="P90" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q90" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T90" s="2" t="s">
         <v>463</v>
       </c>
@@ -11545,6 +11805,9 @@
       <c r="P91" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q91" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T91" s="2" t="s">
         <v>471</v>
       </c>
@@ -11598,6 +11861,9 @@
       <c r="P92" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q92" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T92" s="2" t="s">
         <v>120</v>
       </c>
@@ -11651,6 +11917,9 @@
       <c r="P93" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q93" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T93" s="2" t="s">
         <v>476</v>
       </c>
@@ -11704,6 +11973,9 @@
       <c r="P94" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q94" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T94" s="2" t="s">
         <v>471</v>
       </c>
@@ -11757,6 +12029,9 @@
       <c r="P95" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q95" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T95" s="2" t="s">
         <v>484</v>
       </c>
@@ -11810,6 +12085,9 @@
       <c r="P96" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q96" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T96" s="2" t="s">
         <v>492</v>
       </c>
@@ -11863,6 +12141,9 @@
       <c r="P97" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q97" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T97" s="2" t="s">
         <v>113</v>
       </c>
@@ -11916,6 +12197,9 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q98" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T98" s="2" t="s">
         <v>120</v>
       </c>
@@ -11969,6 +12253,9 @@
       <c r="P99" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q99" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T99" s="2" t="s">
         <v>138</v>
       </c>
@@ -12022,6 +12309,9 @@
       <c r="P100" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q100" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T100" s="2" t="s">
         <v>120</v>
       </c>
@@ -12075,6 +12365,9 @@
       <c r="P101" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q101" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T101" s="2" t="s">
         <v>471</v>
       </c>
@@ -12128,6 +12421,9 @@
       <c r="P102" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q102" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T102" s="2" t="s">
         <v>471</v>
       </c>
@@ -12181,6 +12477,9 @@
       <c r="P103" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q103" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T103" s="2" t="s">
         <v>523</v>
       </c>
@@ -12234,6 +12533,9 @@
       <c r="P104" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q104" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T104" s="2" t="s">
         <v>528</v>
       </c>
@@ -12287,6 +12589,9 @@
       <c r="P105" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q105" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T105" s="2" t="s">
         <v>471</v>
       </c>
@@ -12340,6 +12645,9 @@
       <c r="P106" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q106" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T106" s="2" t="s">
         <v>471</v>
       </c>
@@ -12393,6 +12701,9 @@
       <c r="P107" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q107" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T107" s="2" t="s">
         <v>538</v>
       </c>
@@ -12446,6 +12757,9 @@
       <c r="P108" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q108" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T108" s="2" t="s">
         <v>544</v>
       </c>
@@ -12499,6 +12813,9 @@
       <c r="P109" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q109" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T109" s="2" t="s">
         <v>267</v>
       </c>
@@ -12552,6 +12869,9 @@
       <c r="P110" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q110" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T110" s="2" t="s">
         <v>554</v>
       </c>
@@ -12605,6 +12925,9 @@
       <c r="P111" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q111" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T111" s="2" t="s">
         <v>173</v>
       </c>
@@ -12658,6 +12981,9 @@
       <c r="P112" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q112" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T112" s="2" t="s">
         <v>113</v>
       </c>
@@ -12711,6 +13037,9 @@
       <c r="P113" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q113" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T113" s="2" t="s">
         <v>138</v>
       </c>
@@ -12764,6 +13093,9 @@
       <c r="P114" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q114" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T114" s="2" t="s">
         <v>113</v>
       </c>
@@ -12817,6 +13149,9 @@
       <c r="P115" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q115" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T115" s="2" t="s">
         <v>120</v>
       </c>
@@ -12870,6 +13205,9 @@
       <c r="P116" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q116" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T116" s="2" t="s">
         <v>587</v>
       </c>
@@ -12923,6 +13261,9 @@
       <c r="P117" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q117" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T117" s="2" t="s">
         <v>595</v>
       </c>
@@ -12976,6 +13317,9 @@
       <c r="P118" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q118" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T118" s="2" t="s">
         <v>528</v>
       </c>
@@ -13029,6 +13373,9 @@
       <c r="P119" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q119" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T119" s="2" t="s">
         <v>604</v>
       </c>
@@ -13082,6 +13429,9 @@
       <c r="P120" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q120" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T120" s="2" t="s">
         <v>610</v>
       </c>
@@ -13135,6 +13485,9 @@
       <c r="P121" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q121" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T121" s="2" t="s">
         <v>301</v>
       </c>
@@ -13188,6 +13541,9 @@
       <c r="P122" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q122" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T122" s="2" t="s">
         <v>622</v>
       </c>
@@ -13241,6 +13597,9 @@
       <c r="P123" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q123" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T123" s="2" t="s">
         <v>156</v>
       </c>
@@ -13294,6 +13653,9 @@
       <c r="P124" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q124" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T124" s="2" t="s">
         <v>636</v>
       </c>
@@ -13347,6 +13709,9 @@
       <c r="P125" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q125" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T125" s="2" t="s">
         <v>523</v>
       </c>
@@ -13400,6 +13765,9 @@
       <c r="P126" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q126" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T126" s="2" t="s">
         <v>636</v>
       </c>
@@ -13453,6 +13821,9 @@
       <c r="P127" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q127" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T127" s="2" t="s">
         <v>156</v>
       </c>
@@ -13506,6 +13877,9 @@
       <c r="P128" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q128" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T128" s="2" t="s">
         <v>587</v>
       </c>
@@ -13559,6 +13933,9 @@
       <c r="P129" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q129" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T129" s="2" t="s">
         <v>656</v>
       </c>
@@ -13612,6 +13989,9 @@
       <c r="P130" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q130" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T130" s="2" t="s">
         <v>664</v>
       </c>
@@ -13665,6 +14045,9 @@
       <c r="P131" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q131" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T131" s="2" t="s">
         <v>669</v>
       </c>
@@ -13718,6 +14101,9 @@
       <c r="P132" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q132" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T132" s="2" t="s">
         <v>674</v>
       </c>
@@ -13771,6 +14157,9 @@
       <c r="P133" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q133" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T133" s="2" t="s">
         <v>681</v>
       </c>
@@ -13824,6 +14213,9 @@
       <c r="P134" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q134" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T134" s="2" t="s">
         <v>687</v>
       </c>
@@ -13877,6 +14269,9 @@
       <c r="P135" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q135" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T135" s="2" t="s">
         <v>692</v>
       </c>
@@ -13930,6 +14325,9 @@
       <c r="P136" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q136" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T136" s="7" t="s">
         <v>699</v>
       </c>
@@ -13983,6 +14381,9 @@
       <c r="P137" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q137" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T137" s="2" t="s">
         <v>705</v>
       </c>
@@ -14036,6 +14437,9 @@
       <c r="P138" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q138" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T138" s="2" t="s">
         <v>712</v>
       </c>
@@ -14089,6 +14493,9 @@
       <c r="P139" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q139" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T139" s="2" t="s">
         <v>719</v>
       </c>
@@ -14142,6 +14549,9 @@
       <c r="P140" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q140" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T140" s="2" t="s">
         <v>725</v>
       </c>
@@ -14195,6 +14605,9 @@
       <c r="P141" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q141" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T141" s="2" t="s">
         <v>719</v>
       </c>
@@ -14248,6 +14661,9 @@
       <c r="P142" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q142" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T142" s="2" t="s">
         <v>725</v>
       </c>
@@ -14301,6 +14717,9 @@
       <c r="P143" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q143" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T143" s="2" t="s">
         <v>744</v>
       </c>
@@ -14354,6 +14773,9 @@
       <c r="P144" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q144" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T144" s="2" t="s">
         <v>744</v>
       </c>
@@ -14407,6 +14829,9 @@
       <c r="P145" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q145" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T145" s="2" t="s">
         <v>744</v>
       </c>
@@ -14460,6 +14885,9 @@
       <c r="P146" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q146" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T146" s="2" t="s">
         <v>744</v>
       </c>
@@ -14513,6 +14941,9 @@
       <c r="P147" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q147" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T147" s="2" t="s">
         <v>744</v>
       </c>
@@ -14566,6 +14997,9 @@
       <c r="P148" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q148" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T148" s="2" t="s">
         <v>773</v>
       </c>
@@ -14619,6 +15053,9 @@
       <c r="P149" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q149" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T149" s="2" t="s">
         <v>779</v>
       </c>
@@ -14672,6 +15109,9 @@
       <c r="P150" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q150" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T150" s="2" t="s">
         <v>674</v>
       </c>
@@ -14725,6 +15165,9 @@
       <c r="P151" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q151" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T151" s="2" t="s">
         <v>773</v>
       </c>
@@ -14778,6 +15221,9 @@
       <c r="P152" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q152" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T152" s="2" t="s">
         <v>792</v>
       </c>
@@ -14831,6 +15277,9 @@
       <c r="P153" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q153" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T153" s="2" t="s">
         <v>798</v>
       </c>
@@ -14881,6 +15330,9 @@
       <c r="P154" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q154" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T154" s="2" t="s">
         <v>806</v>
       </c>
@@ -14934,6 +15386,9 @@
       <c r="P155" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q155" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T155" s="2" t="s">
         <v>813</v>
       </c>
@@ -14987,6 +15442,9 @@
       <c r="P156" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q156" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T156" s="2" t="s">
         <v>818</v>
       </c>
@@ -15041,6 +15499,9 @@
       <c r="P157" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q157" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T157" s="2" t="s">
         <v>823</v>
       </c>
@@ -15095,6 +15556,9 @@
       <c r="P158" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q158" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T158" s="2" t="s">
         <v>827</v>
       </c>
@@ -15149,6 +15613,9 @@
       <c r="P159" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q159" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T159" s="2" t="s">
         <v>835</v>
       </c>
@@ -15203,6 +15670,9 @@
       <c r="P160" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q160" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T160" s="2" t="s">
         <v>841</v>
       </c>
@@ -15257,6 +15727,9 @@
       <c r="P161" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q161" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T161" s="2" t="s">
         <v>847</v>
       </c>
@@ -15311,6 +15784,9 @@
       <c r="P162" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q162" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T162" s="2" t="s">
         <v>853</v>
       </c>
@@ -15365,6 +15841,9 @@
       <c r="P163" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q163" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T163" s="2" t="s">
         <v>859</v>
       </c>
@@ -15418,6 +15897,9 @@
       <c r="P164" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q164" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T164" s="2" t="s">
         <v>865</v>
       </c>
@@ -15471,6 +15953,9 @@
       <c r="P165" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q165" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T165" s="2" t="s">
         <v>873</v>
       </c>
@@ -15524,6 +16009,9 @@
       <c r="P166" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q166" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T166" s="2" t="s">
         <v>879</v>
       </c>
@@ -15577,6 +16065,9 @@
       <c r="P167" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q167" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T167" s="2" t="s">
         <v>886</v>
       </c>
@@ -15630,6 +16121,9 @@
       <c r="P168" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q168" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T168" s="2" t="s">
         <v>891</v>
       </c>
@@ -15683,6 +16177,9 @@
       <c r="P169" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q169" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T169" s="2" t="s">
         <v>897</v>
       </c>
@@ -15736,6 +16233,9 @@
       <c r="P170" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q170" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T170" s="2" t="s">
         <v>899</v>
       </c>
@@ -15789,6 +16289,9 @@
       <c r="P171" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q171" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T171" s="2" t="s">
         <v>901</v>
       </c>
@@ -15842,6 +16345,9 @@
       <c r="P172" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q172" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T172" s="2" t="s">
         <v>908</v>
       </c>
@@ -15895,6 +16401,9 @@
       <c r="P173" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q173" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T173" s="2" t="s">
         <v>915</v>
       </c>
@@ -15948,6 +16457,9 @@
       <c r="P174" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q174" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T174" s="2" t="s">
         <v>921</v>
       </c>
@@ -15998,6 +16510,9 @@
       <c r="P175" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q175" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T175" s="2" t="s">
         <v>925</v>
       </c>
@@ -16051,6 +16566,9 @@
       <c r="P176" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q176" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T176" s="2" t="s">
         <v>931</v>
       </c>
@@ -16104,6 +16622,9 @@
       <c r="P177" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q177" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T177" s="2" t="s">
         <v>938</v>
       </c>
@@ -16158,6 +16679,9 @@
       <c r="P178" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q178" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T178" s="2" t="s">
         <v>945</v>
       </c>
@@ -16212,6 +16736,9 @@
       <c r="P179" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q179" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T179" s="2" t="s">
         <v>951</v>
       </c>
@@ -16267,7 +16794,9 @@
       <c r="P180" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q180" s="7"/>
+      <c r="Q180" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R180" s="7"/>
       <c r="S180" s="7"/>
       <c r="T180" s="7" t="s">
@@ -16330,7 +16859,9 @@
       <c r="P181" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q181" s="7"/>
+      <c r="Q181" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="R181" s="7"/>
       <c r="S181" s="7"/>
       <c r="T181" s="7" t="s">
@@ -16391,6 +16922,9 @@
       <c r="P182" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q182" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T182" s="7" t="s">
         <v>970</v>
       </c>
@@ -16444,6 +16978,9 @@
       <c r="P183" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q183" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T183" s="7" t="s">
         <v>977</v>
       </c>
@@ -16497,6 +17034,9 @@
       <c r="P184" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q184" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T184" s="7" t="s">
         <v>983</v>
       </c>
@@ -16550,6 +17090,9 @@
       <c r="P185" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q185" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T185" s="2" t="s">
         <v>992</v>
       </c>
@@ -16603,6 +17146,9 @@
       <c r="P186" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q186" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T186" s="2" t="s">
         <v>998</v>
       </c>
@@ -16656,6 +17202,9 @@
       <c r="P187" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q187" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T187" s="2" t="s">
         <v>1004</v>
       </c>
@@ -16709,6 +17258,9 @@
       <c r="P188" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q188" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T188" s="2" t="s">
         <v>1006</v>
       </c>
@@ -16762,6 +17314,9 @@
       <c r="P189" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q189" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T189" s="2" t="s">
         <v>1008</v>
       </c>
@@ -16815,6 +17370,9 @@
       <c r="P190" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q190" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T190" s="2" t="s">
         <v>1013</v>
       </c>
@@ -16868,6 +17426,9 @@
       <c r="P191" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q191" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T191" s="2" t="s">
         <v>1018</v>
       </c>
@@ -16921,6 +17482,9 @@
       <c r="P192" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q192" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T192" s="2" t="s">
         <v>1024</v>
       </c>
@@ -16974,6 +17538,9 @@
       <c r="P193" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q193" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T193" s="2" t="s">
         <v>1030</v>
       </c>
@@ -17027,6 +17594,9 @@
       <c r="P194" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q194" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T194" s="2" t="s">
         <v>1035</v>
       </c>
@@ -17080,6 +17650,9 @@
       <c r="P195" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q195" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T195" s="2" t="s">
         <v>1040</v>
       </c>
@@ -17133,6 +17706,9 @@
       <c r="P196" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q196" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T196" s="2" t="s">
         <v>1045</v>
       </c>
@@ -17186,6 +17762,9 @@
       <c r="P197" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q197" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T197" s="2" t="s">
         <v>1052</v>
       </c>
@@ -17239,6 +17818,9 @@
       <c r="P198" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q198" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T198" s="2" t="s">
         <v>1058</v>
       </c>
@@ -17292,6 +17874,9 @@
       <c r="P199" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q199" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T199" s="2" t="s">
         <v>1065</v>
       </c>
@@ -17345,6 +17930,9 @@
       <c r="P200" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q200" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T200" s="2" t="s">
         <v>1071</v>
       </c>
@@ -17398,6 +17986,9 @@
       <c r="P201" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q201" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T201" s="2" t="s">
         <v>1076</v>
       </c>
@@ -17451,6 +18042,9 @@
       <c r="P202" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q202" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T202" s="2" t="s">
         <v>1082</v>
       </c>
@@ -17504,6 +18098,9 @@
       <c r="P203" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q203" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T203" s="2" t="s">
         <v>1090</v>
       </c>
@@ -17557,6 +18154,9 @@
       <c r="P204" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q204" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T204" s="2" t="s">
         <v>1095</v>
       </c>
@@ -17610,6 +18210,9 @@
       <c r="P205" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q205" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T205" s="2" t="s">
         <v>1098</v>
       </c>
@@ -17663,6 +18266,9 @@
       <c r="P206" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q206" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T206" s="2" t="s">
         <v>1100</v>
       </c>
@@ -17716,6 +18322,9 @@
       <c r="P207" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q207" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T207" s="2" t="s">
         <v>1105</v>
       </c>
@@ -17769,6 +18378,9 @@
       <c r="P208" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q208" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T208" s="2" t="s">
         <v>1109</v>
       </c>
@@ -17822,6 +18434,9 @@
       <c r="P209" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q209" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T209" s="2" t="s">
         <v>1113</v>
       </c>
@@ -17875,6 +18490,9 @@
       <c r="P210" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q210" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T210" s="2" t="s">
         <v>1118</v>
       </c>
@@ -17928,6 +18546,9 @@
       <c r="P211" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q211" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T211" s="2" t="s">
         <v>1125</v>
       </c>
@@ -17981,6 +18602,9 @@
       <c r="P212" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q212" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T212" s="2" t="s">
         <v>1136</v>
       </c>
@@ -18034,6 +18658,9 @@
       <c r="P213" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q213" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T213" s="2" t="s">
         <v>1143</v>
       </c>
@@ -18087,6 +18714,9 @@
       <c r="P214" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q214" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T214" s="2" t="s">
         <v>1149</v>
       </c>
@@ -18140,6 +18770,9 @@
       <c r="P215" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q215" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T215" s="2" t="s">
         <v>1154</v>
       </c>
@@ -18193,6 +18826,9 @@
       <c r="P216" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q216" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T216" s="2" t="s">
         <v>1161</v>
       </c>
@@ -18246,6 +18882,9 @@
       <c r="P217" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q217" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T217" s="2" t="s">
         <v>1165</v>
       </c>
@@ -18299,6 +18938,9 @@
       <c r="P218" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q218" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T218" s="2" t="s">
         <v>1170</v>
       </c>
@@ -18352,6 +18994,9 @@
       <c r="P219" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q219" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T219" s="2" t="s">
         <v>1165</v>
       </c>
@@ -18405,6 +19050,9 @@
       <c r="P220" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q220" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T220" s="2" t="s">
         <v>1181</v>
       </c>
@@ -18458,6 +19106,9 @@
       <c r="P221" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q221" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T221" s="2" t="s">
         <v>1187</v>
       </c>
@@ -18511,6 +19162,9 @@
       <c r="P222" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q222" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T222" s="2" t="s">
         <v>1194</v>
       </c>
@@ -18564,6 +19218,9 @@
       <c r="P223" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q223" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T223" s="2" t="s">
         <v>1200</v>
       </c>
@@ -18617,6 +19274,9 @@
       <c r="P224" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q224" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T224" s="2" t="s">
         <v>1200</v>
       </c>
@@ -18670,6 +19330,9 @@
       <c r="P225" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q225" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T225" s="2" t="s">
         <v>1213</v>
       </c>
@@ -18723,6 +19386,9 @@
       <c r="P226" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q226" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T226" s="2" t="s">
         <v>1220</v>
       </c>
@@ -18776,6 +19442,9 @@
       <c r="P227" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q227" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T227" s="2" t="s">
         <v>1213</v>
       </c>
@@ -18829,6 +19498,9 @@
       <c r="P228" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q228" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T228" s="2" t="s">
         <v>1231</v>
       </c>
@@ -18882,6 +19554,9 @@
       <c r="P229" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q229" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T229" s="2" t="s">
         <v>1237</v>
       </c>
@@ -18935,6 +19610,9 @@
       <c r="P230" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q230" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T230" s="2" t="s">
         <v>1245</v>
       </c>
@@ -18988,6 +19666,9 @@
       <c r="P231" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q231" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T231" s="2" t="s">
         <v>1245</v>
       </c>
@@ -19041,6 +19722,9 @@
       <c r="P232" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q232" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T232" s="2" t="s">
         <v>1245</v>
       </c>
@@ -19094,6 +19778,9 @@
       <c r="P233" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q233" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T233" s="2" t="s">
         <v>1245</v>
       </c>
@@ -19147,6 +19834,9 @@
       <c r="P234" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q234" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T234" s="2" t="s">
         <v>1245</v>
       </c>
@@ -19200,6 +19890,9 @@
       <c r="P235" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q235" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T235" s="2" t="s">
         <v>1275</v>
       </c>
@@ -19253,6 +19946,9 @@
       <c r="P236" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q236" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T236" s="2" t="s">
         <v>1281</v>
       </c>
@@ -19306,6 +20002,9 @@
       <c r="P237" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q237" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T237" s="2" t="s">
         <v>1287</v>
       </c>
@@ -19359,6 +20058,9 @@
       <c r="P238" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q238" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T238" s="2" t="s">
         <v>179</v>
       </c>
@@ -19412,6 +20114,9 @@
       <c r="P239" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q239" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T239" s="2" t="s">
         <v>1275</v>
       </c>
@@ -19465,6 +20170,9 @@
       <c r="P240" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q240" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T240" s="2" t="s">
         <v>1306</v>
       </c>
@@ -19515,6 +20223,9 @@
       <c r="P241" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q241" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T241" s="2" t="s">
         <v>1312</v>
       </c>
@@ -19565,6 +20276,9 @@
       <c r="P242" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q242" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T242" s="2" t="s">
         <v>179</v>
       </c>
@@ -19615,6 +20329,9 @@
       <c r="P243" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q243" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T243" s="2" t="s">
         <v>1149</v>
       </c>
@@ -19665,6 +20382,9 @@
       <c r="P244" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q244" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T244" s="2" t="s">
         <v>179</v>
       </c>
@@ -19715,6 +20435,9 @@
       <c r="P245" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q245" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T245" s="2" t="s">
         <v>138</v>
       </c>
@@ -19765,6 +20488,9 @@
       <c r="P246" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q246" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T246" s="2" t="s">
         <v>1336</v>
       </c>
@@ -19815,6 +20541,9 @@
       <c r="P247" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q247" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T247" s="2" t="s">
         <v>1344</v>
       </c>
@@ -19865,6 +20594,9 @@
       <c r="P248" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q248" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T248" s="2" t="s">
         <v>1349</v>
       </c>
@@ -19915,6 +20647,9 @@
       <c r="P249" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q249" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T249" s="2" t="s">
         <v>1306</v>
       </c>
@@ -19965,6 +20700,9 @@
       <c r="P250" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q250" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T250" s="2" t="s">
         <v>1360</v>
       </c>
@@ -20015,6 +20753,9 @@
       <c r="P251" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="Q251" s="2" t="n">
+        <v>999999</v>
+      </c>
       <c r="T251" s="2" t="s">
         <v>179</v>
       </c>
@@ -20063,7 +20804,7 @@
         <v>0</v>
       </c>
       <c r="Q252" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R252" s="2" t="s">
         <v>1371</v>
@@ -20122,7 +20863,7 @@
         <v>0</v>
       </c>
       <c r="Q253" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R253" s="2" t="s">
         <v>1371</v>
@@ -20181,7 +20922,7 @@
         <v>0</v>
       </c>
       <c r="Q254" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R254" s="2" t="s">
         <v>1371</v>
@@ -20240,7 +20981,7 @@
         <v>0</v>
       </c>
       <c r="Q255" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R255" s="2" t="s">
         <v>1371</v>
@@ -20299,7 +21040,7 @@
         <v>0</v>
       </c>
       <c r="Q256" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R256" s="2" t="s">
         <v>1371</v>
@@ -20358,7 +21099,7 @@
         <v>0</v>
       </c>
       <c r="Q257" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R257" s="2" t="s">
         <v>1371</v>
@@ -20417,7 +21158,7 @@
         <v>0</v>
       </c>
       <c r="Q258" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R258" s="2" t="s">
         <v>1371</v>
@@ -20476,7 +21217,7 @@
         <v>0</v>
       </c>
       <c r="Q259" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R259" s="2" t="s">
         <v>1371</v>
@@ -20535,7 +21276,7 @@
         <v>0</v>
       </c>
       <c r="Q260" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R260" s="2" t="s">
         <v>1371</v>
@@ -20594,7 +21335,7 @@
         <v>0</v>
       </c>
       <c r="Q261" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R261" s="2" t="s">
         <v>1371</v>
@@ -20653,7 +21394,7 @@
         <v>0</v>
       </c>
       <c r="Q262" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R262" s="2" t="s">
         <v>1371</v>
@@ -20712,7 +21453,7 @@
         <v>0</v>
       </c>
       <c r="Q263" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R263" s="2" t="s">
         <v>1371</v>
@@ -20771,7 +21512,7 @@
         <v>0</v>
       </c>
       <c r="Q264" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R264" s="2" t="s">
         <v>1371</v>
@@ -20830,7 +21571,7 @@
         <v>0</v>
       </c>
       <c r="Q265" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R265" s="2" t="s">
         <v>1371</v>
@@ -20889,7 +21630,7 @@
         <v>0</v>
       </c>
       <c r="Q266" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R266" s="2" t="s">
         <v>1371</v>
@@ -20948,7 +21689,7 @@
         <v>0</v>
       </c>
       <c r="Q267" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R267" s="2" t="s">
         <v>1371</v>
@@ -21007,7 +21748,7 @@
         <v>0</v>
       </c>
       <c r="Q268" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R268" s="2" t="s">
         <v>1371</v>
@@ -21066,7 +21807,7 @@
         <v>0</v>
       </c>
       <c r="Q269" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R269" s="2" t="s">
         <v>1470</v>
@@ -21125,7 +21866,7 @@
         <v>0</v>
       </c>
       <c r="Q270" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R270" s="2" t="s">
         <v>1470</v>
@@ -21184,7 +21925,7 @@
         <v>0</v>
       </c>
       <c r="Q271" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R271" s="2" t="s">
         <v>1470</v>
@@ -21243,7 +21984,7 @@
         <v>0</v>
       </c>
       <c r="Q272" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R272" s="2" t="s">
         <v>1470</v>
@@ -21302,7 +22043,7 @@
         <v>0</v>
       </c>
       <c r="Q273" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R273" s="2" t="s">
         <v>1470</v>
@@ -21361,7 +22102,7 @@
         <v>0</v>
       </c>
       <c r="Q274" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R274" s="2" t="s">
         <v>1470</v>
@@ -21420,7 +22161,7 @@
         <v>0</v>
       </c>
       <c r="Q275" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R275" s="2" t="s">
         <v>1504</v>
@@ -21479,7 +22220,7 @@
         <v>0</v>
       </c>
       <c r="Q276" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R276" s="2" t="s">
         <v>1504</v>
@@ -21538,7 +22279,7 @@
         <v>0</v>
       </c>
       <c r="Q277" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R277" s="2" t="s">
         <v>1470</v>
@@ -21594,7 +22335,7 @@
         <v>0</v>
       </c>
       <c r="Q278" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R278" s="2" t="s">
         <v>1470</v>
@@ -21650,7 +22391,7 @@
         <v>0</v>
       </c>
       <c r="Q279" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R279" s="2" t="s">
         <v>1470</v>
@@ -21706,7 +22447,7 @@
         <v>0</v>
       </c>
       <c r="Q280" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R280" s="2" t="s">
         <v>1504</v>
@@ -21762,7 +22503,7 @@
         <v>0</v>
       </c>
       <c r="Q281" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R281" s="2" t="s">
         <v>1504</v>
@@ -21821,7 +22562,7 @@
         <v>0</v>
       </c>
       <c r="Q282" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R282" s="2" t="s">
         <v>1470</v>
@@ -21880,7 +22621,7 @@
         <v>0</v>
       </c>
       <c r="Q283" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R283" s="2" t="s">
         <v>1470</v>
@@ -21939,7 +22680,7 @@
         <v>0</v>
       </c>
       <c r="Q284" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R284" s="2" t="s">
         <v>1504</v>
@@ -21998,7 +22739,7 @@
         <v>0</v>
       </c>
       <c r="Q285" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R285" s="2" t="s">
         <v>1504</v>
@@ -22057,7 +22798,7 @@
         <v>0</v>
       </c>
       <c r="Q286" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R286" s="2" t="s">
         <v>1470</v>
@@ -22116,7 +22857,7 @@
         <v>0</v>
       </c>
       <c r="Q287" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R287" s="2" t="s">
         <v>1470</v>
@@ -22175,7 +22916,7 @@
         <v>0</v>
       </c>
       <c r="Q288" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R288" s="2" t="s">
         <v>1504</v>
@@ -22234,7 +22975,7 @@
         <v>0</v>
       </c>
       <c r="Q289" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R289" s="2" t="s">
         <v>1504</v>
@@ -22293,7 +23034,7 @@
         <v>0</v>
       </c>
       <c r="Q290" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R290" s="2" t="s">
         <v>1470</v>
@@ -22352,7 +23093,7 @@
         <v>0</v>
       </c>
       <c r="Q291" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R291" s="2" t="s">
         <v>1504</v>
@@ -22411,7 +23152,7 @@
         <v>0</v>
       </c>
       <c r="Q292" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R292" s="2" t="s">
         <v>1470</v>
@@ -22470,7 +23211,7 @@
         <v>0</v>
       </c>
       <c r="Q293" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R293" s="2" t="s">
         <v>1504</v>
@@ -22529,7 +23270,7 @@
         <v>0</v>
       </c>
       <c r="Q294" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R294" s="2" t="s">
         <v>1470</v>
@@ -22588,7 +23329,7 @@
         <v>0</v>
       </c>
       <c r="Q295" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R295" s="2" t="s">
         <v>1504</v>
@@ -22647,7 +23388,7 @@
         <v>0</v>
       </c>
       <c r="Q296" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R296" s="2" t="s">
         <v>1371</v>
@@ -22706,7 +23447,7 @@
         <v>0</v>
       </c>
       <c r="Q297" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R297" s="2" t="s">
         <v>1371</v>
@@ -22765,7 +23506,7 @@
         <v>0</v>
       </c>
       <c r="Q298" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R298" s="2" t="s">
         <v>1371</v>
@@ -22824,7 +23565,7 @@
         <v>0</v>
       </c>
       <c r="Q299" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R299" s="2" t="s">
         <v>1371</v>
@@ -22883,7 +23624,7 @@
         <v>0</v>
       </c>
       <c r="Q300" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R300" s="2" t="s">
         <v>1371</v>
@@ -22942,7 +23683,7 @@
         <v>0</v>
       </c>
       <c r="Q301" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R301" s="2" t="s">
         <v>1371</v>
@@ -23001,7 +23742,7 @@
         <v>0</v>
       </c>
       <c r="Q302" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R302" s="2" t="s">
         <v>1371</v>
@@ -23060,7 +23801,7 @@
         <v>0</v>
       </c>
       <c r="Q303" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R303" s="2" t="s">
         <v>1611</v>
@@ -23116,7 +23857,7 @@
         <v>0</v>
       </c>
       <c r="Q304" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R304" s="2" t="s">
         <v>1371</v>
@@ -23172,7 +23913,7 @@
         <v>0</v>
       </c>
       <c r="Q305" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R305" s="2" t="s">
         <v>1470</v>
@@ -23231,7 +23972,7 @@
         <v>0</v>
       </c>
       <c r="Q306" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R306" s="2" t="s">
         <v>1611</v>
@@ -23290,7 +24031,7 @@
         <v>0</v>
       </c>
       <c r="Q307" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R307" s="2" t="s">
         <v>1611</v>
@@ -23346,7 +24087,7 @@
         <v>0</v>
       </c>
       <c r="Q308" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R308" s="2" t="s">
         <v>1470</v>
@@ -23405,7 +24146,7 @@
         <v>0</v>
       </c>
       <c r="Q309" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R309" s="2" t="s">
         <v>1470</v>
@@ -23464,7 +24205,7 @@
         <v>0</v>
       </c>
       <c r="Q310" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R310" s="2" t="s">
         <v>1371</v>
@@ -23523,7 +24264,7 @@
         <v>0</v>
       </c>
       <c r="Q311" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R311" s="2" t="s">
         <v>1371</v>
@@ -23582,7 +24323,7 @@
         <v>0</v>
       </c>
       <c r="Q312" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R312" s="2" t="s">
         <v>1371</v>
@@ -23641,7 +24382,7 @@
         <v>0</v>
       </c>
       <c r="Q313" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R313" s="2" t="s">
         <v>1371</v>
@@ -23700,7 +24441,7 @@
         <v>0</v>
       </c>
       <c r="Q314" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R314" s="2" t="s">
         <v>1371</v>
@@ -23759,7 +24500,7 @@
         <v>0</v>
       </c>
       <c r="Q315" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R315" s="2" t="s">
         <v>1371</v>
@@ -23818,7 +24559,7 @@
         <v>0</v>
       </c>
       <c r="Q316" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R316" s="2" t="s">
         <v>1371</v>
@@ -23877,7 +24618,7 @@
         <v>0</v>
       </c>
       <c r="Q317" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R317" s="2" t="s">
         <v>1611</v>
@@ -23936,7 +24677,7 @@
         <v>0</v>
       </c>
       <c r="Q318" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R318" s="2" t="s">
         <v>1371</v>
@@ -23995,7 +24736,7 @@
         <v>0</v>
       </c>
       <c r="Q319" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R319" s="2" t="s">
         <v>1371</v>
@@ -24051,7 +24792,7 @@
         <v>0</v>
       </c>
       <c r="Q320" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R320" s="2" t="s">
         <v>1371</v>
@@ -24110,7 +24851,7 @@
         <v>0</v>
       </c>
       <c r="Q321" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R321" s="2" t="s">
         <v>1371</v>
@@ -24169,7 +24910,7 @@
         <v>0</v>
       </c>
       <c r="Q322" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R322" s="2" t="s">
         <v>1371</v>
@@ -24228,7 +24969,7 @@
         <v>0</v>
       </c>
       <c r="Q323" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R323" s="2" t="s">
         <v>1371</v>
@@ -24287,7 +25028,7 @@
         <v>0</v>
       </c>
       <c r="Q324" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R324" s="2" t="s">
         <v>1371</v>
@@ -24343,7 +25084,7 @@
         <v>0</v>
       </c>
       <c r="Q325" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R325" s="2" t="s">
         <v>1371</v>
@@ -24399,7 +25140,7 @@
         <v>0</v>
       </c>
       <c r="Q326" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R326" s="2" t="s">
         <v>1371</v>
@@ -24458,7 +25199,7 @@
         <v>0</v>
       </c>
       <c r="Q327" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R327" s="2" t="s">
         <v>1371</v>
@@ -24517,7 +25258,7 @@
         <v>0</v>
       </c>
       <c r="Q328" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R328" s="2" t="s">
         <v>1611</v>
@@ -24573,7 +25314,7 @@
         <v>0</v>
       </c>
       <c r="Q329" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R329" s="2" t="s">
         <v>1371</v>
@@ -24632,7 +25373,7 @@
         <v>0</v>
       </c>
       <c r="Q330" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R330" s="2" t="s">
         <v>1371</v>
@@ -24691,7 +25432,7 @@
         <v>0</v>
       </c>
       <c r="Q331" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R331" s="2" t="s">
         <v>1770</v>
@@ -24750,7 +25491,7 @@
         <v>0</v>
       </c>
       <c r="Q332" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R332" s="2" t="s">
         <v>1371</v>
@@ -24809,7 +25550,7 @@
         <v>0</v>
       </c>
       <c r="Q333" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R333" s="2" t="s">
         <v>1371</v>
@@ -24868,7 +25609,7 @@
         <v>0</v>
       </c>
       <c r="Q334" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R334" s="2" t="s">
         <v>1371</v>
@@ -24927,7 +25668,7 @@
         <v>0</v>
       </c>
       <c r="Q335" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R335" s="2" t="s">
         <v>1371</v>
@@ -24983,7 +25724,7 @@
         <v>0</v>
       </c>
       <c r="Q336" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R336" s="2" t="s">
         <v>1470</v>
@@ -25039,7 +25780,7 @@
         <v>0</v>
       </c>
       <c r="Q337" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R337" s="2" t="s">
         <v>1470</v>
@@ -25095,7 +25836,7 @@
         <v>0</v>
       </c>
       <c r="Q338" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R338" s="2" t="s">
         <v>1807</v>
@@ -25154,7 +25895,7 @@
         <v>0</v>
       </c>
       <c r="Q339" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="U339" s="2" t="s">
         <v>1813</v>
@@ -25204,7 +25945,7 @@
         <v>0</v>
       </c>
       <c r="Q340" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R340" s="2" t="s">
         <v>1817</v>
@@ -25263,7 +26004,7 @@
         <v>0</v>
       </c>
       <c r="Q341" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R341" s="2" t="s">
         <v>1371</v>
@@ -25322,7 +26063,7 @@
         <v>0</v>
       </c>
       <c r="Q342" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R342" s="2" t="s">
         <v>1371</v>
@@ -25381,7 +26122,7 @@
         <v>0</v>
       </c>
       <c r="Q343" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R343" s="2" t="s">
         <v>1371</v>
@@ -25440,7 +26181,7 @@
         <v>0</v>
       </c>
       <c r="Q344" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R344" s="2" t="s">
         <v>1843</v>
@@ -25496,7 +26237,7 @@
         <v>0</v>
       </c>
       <c r="Q345" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R345" s="2" t="s">
         <v>1843</v>
@@ -25555,7 +26296,7 @@
         <v>0</v>
       </c>
       <c r="Q346" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R346" s="2" t="s">
         <v>1855</v>
@@ -25614,7 +26355,7 @@
         <v>0</v>
       </c>
       <c r="Q347" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R347" s="2" t="s">
         <v>1470</v>
@@ -25673,7 +26414,7 @@
         <v>0</v>
       </c>
       <c r="Q348" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R348" s="2" t="s">
         <v>1470</v>
@@ -25732,7 +26473,7 @@
         <v>0</v>
       </c>
       <c r="Q349" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R349" s="2" t="s">
         <v>1470</v>
@@ -25791,7 +26532,7 @@
         <v>0</v>
       </c>
       <c r="Q350" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R350" s="2" t="s">
         <v>1470</v>
@@ -25850,7 +26591,7 @@
         <v>0</v>
       </c>
       <c r="Q351" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R351" s="2" t="s">
         <v>1889</v>
@@ -25909,7 +26650,7 @@
         <v>0</v>
       </c>
       <c r="Q352" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R352" s="2" t="s">
         <v>1470</v>
@@ -25968,7 +26709,7 @@
         <v>0</v>
       </c>
       <c r="Q353" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R353" s="2" t="s">
         <v>1371</v>
@@ -26027,7 +26768,7 @@
         <v>0</v>
       </c>
       <c r="Q354" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R354" s="2" t="s">
         <v>1371</v>
@@ -26086,7 +26827,7 @@
         <v>0</v>
       </c>
       <c r="Q355" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="T355" s="2" t="s">
         <v>1170</v>
@@ -26142,7 +26883,7 @@
         <v>0</v>
       </c>
       <c r="Q356" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R356" s="2" t="s">
         <v>1470</v>
@@ -26201,7 +26942,7 @@
         <v>0</v>
       </c>
       <c r="Q357" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R357" s="2" t="s">
         <v>1470</v>
@@ -26257,7 +26998,7 @@
         <v>0</v>
       </c>
       <c r="Q358" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R358" s="2" t="s">
         <v>1843</v>
@@ -26310,7 +27051,7 @@
         <v>0</v>
       </c>
       <c r="Q359" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R359" s="2" t="s">
         <v>1470</v>
@@ -26369,7 +27110,7 @@
         <v>0</v>
       </c>
       <c r="Q360" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R360" s="2" t="s">
         <v>1470</v>
@@ -26428,7 +27169,7 @@
         <v>0</v>
       </c>
       <c r="Q361" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R361" s="2" t="s">
         <v>1470</v>
@@ -26487,7 +27228,7 @@
         <v>0</v>
       </c>
       <c r="Q362" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R362" s="2" t="s">
         <v>1956</v>
@@ -26546,7 +27287,7 @@
         <v>0</v>
       </c>
       <c r="Q363" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R363" s="2" t="s">
         <v>1470</v>
@@ -26602,7 +27343,7 @@
         <v>0</v>
       </c>
       <c r="Q364" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R364" s="2" t="s">
         <v>1371</v>
@@ -26658,7 +27399,7 @@
         <v>0</v>
       </c>
       <c r="Q365" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R365" s="2" t="s">
         <v>1371</v>
@@ -26714,7 +27455,7 @@
         <v>0</v>
       </c>
       <c r="Q366" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R366" s="2" t="s">
         <v>1371</v>
@@ -26770,7 +27511,7 @@
         <v>0</v>
       </c>
       <c r="Q367" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R367" s="2" t="s">
         <v>1981</v>
@@ -26829,7 +27570,7 @@
         <v>0</v>
       </c>
       <c r="Q368" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R368" s="2" t="s">
         <v>1981</v>
@@ -26888,7 +27629,7 @@
         <v>0</v>
       </c>
       <c r="Q369" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R369" s="2" t="s">
         <v>1371</v>
@@ -26947,7 +27688,7 @@
         <v>0</v>
       </c>
       <c r="Q370" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R370" s="2" t="s">
         <v>1470</v>
@@ -27006,7 +27747,7 @@
         <v>0</v>
       </c>
       <c r="Q371" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R371" s="2" t="s">
         <v>1470</v>
@@ -27065,7 +27806,7 @@
         <v>0</v>
       </c>
       <c r="Q372" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R372" s="2" t="s">
         <v>1470</v>
@@ -27121,7 +27862,7 @@
         <v>0</v>
       </c>
       <c r="Q373" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R373" s="2" t="s">
         <v>1470</v>
@@ -27177,7 +27918,7 @@
         <v>0</v>
       </c>
       <c r="Q374" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R374" s="2" t="s">
         <v>1470</v>
@@ -27236,7 +27977,7 @@
         <v>0</v>
       </c>
       <c r="Q375" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R375" s="2" t="s">
         <v>1504</v>
@@ -27295,7 +28036,7 @@
         <v>0</v>
       </c>
       <c r="Q376" s="2" t="n">
-        <v>100</v>
+        <v>999999</v>
       </c>
       <c r="R376" s="2" t="s">
         <v>1470</v>

</xml_diff>